<commit_message>
matching with pylint and start with subprocess
</commit_message>
<xml_diff>
--- a/bot/data.xlsx
+++ b/bot/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="9">
   <si>
     <t>محمد حسین خادمی</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D200"/>
+  <dimension ref="A1:D270"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="D239" sqref="D239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -385,11 +385,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" t="s">
+        <v>5</v>
       </c>
       <c r="B1">
-        <v>1234567890</v>
+        <v>1234567911</v>
       </c>
       <c r="C1">
         <v>9</v>
@@ -399,11 +399,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>3861802317</v>
+        <v>1234567912</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -414,10 +414,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1234567891</v>
+        <v>1234567913</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -427,11 +427,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
-        <v>1234567892</v>
+        <v>1234567914</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -441,11 +441,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1234567893</v>
+        <v>1234567915</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -455,11 +455,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
+      <c r="A6" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1234567894</v>
+        <v>1234567916</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>1234567895</v>
+        <v>1234567917</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -484,10 +484,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>1234567896</v>
+        <v>1234567918</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -497,11 +497,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>1234567897</v>
+        <v>1234567919</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -511,11 +511,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
+      <c r="A10" t="s">
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>1234567898</v>
+        <v>1234567920</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -525,11 +525,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
+      <c r="A11" t="s">
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>1234567899</v>
+        <v>1234567921</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -540,10 +540,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>1234567900</v>
+        <v>1234567922</v>
       </c>
       <c r="C12">
         <v>9</v>
@@ -553,11 +553,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
+      <c r="A13" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>1234567901</v>
+        <v>1234567923</v>
       </c>
       <c r="C13">
         <v>9</v>
@@ -567,11 +567,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
+      <c r="A14" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B14">
-        <v>1234567902</v>
+        <v>1234567924</v>
       </c>
       <c r="C14">
         <v>9</v>
@@ -581,11 +581,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>6</v>
+      <c r="A15" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>1234567903</v>
+        <v>1234567925</v>
       </c>
       <c r="C15">
         <v>9</v>
@@ -596,10 +596,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16">
-        <v>1234567904</v>
+        <v>1234567926</v>
       </c>
       <c r="C16">
         <v>9</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>1234567905</v>
+        <v>1234567927</v>
       </c>
       <c r="C17">
         <v>9</v>
@@ -623,11 +623,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>8</v>
+      <c r="A18" t="s">
+        <v>4</v>
       </c>
       <c r="B18">
-        <v>1234567906</v>
+        <v>1234567928</v>
       </c>
       <c r="C18">
         <v>9</v>
@@ -637,11 +637,11 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
+      <c r="A19" t="s">
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>1234567907</v>
+        <v>1234567929</v>
       </c>
       <c r="C19">
         <v>9</v>
@@ -651,11 +651,11 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
+      <c r="A20" t="s">
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>1234567908</v>
+        <v>1234567930</v>
       </c>
       <c r="C20">
         <v>9</v>
@@ -666,10 +666,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>1234567909</v>
+        <v>1234567931</v>
       </c>
       <c r="C21">
         <v>9</v>
@@ -679,11 +679,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
+      <c r="A22" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>1234567910</v>
+        <v>1234567932</v>
       </c>
       <c r="C22">
         <v>9</v>
@@ -697,13 +697,13 @@
         <v>5</v>
       </c>
       <c r="B23">
-        <v>1234567911</v>
+        <v>1234567933</v>
       </c>
       <c r="C23">
         <v>9</v>
       </c>
       <c r="D23">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,13 +711,13 @@
         <v>6</v>
       </c>
       <c r="B24">
-        <v>1234567912</v>
+        <v>1234567934</v>
       </c>
       <c r="C24">
         <v>9</v>
       </c>
       <c r="D24">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,13 +725,13 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>1234567913</v>
+        <v>1234567935</v>
       </c>
       <c r="C25">
         <v>9</v>
       </c>
       <c r="D25">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -739,13 +739,13 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>1234567914</v>
+        <v>1234567936</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
       <c r="D26">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,13 +753,13 @@
         <v>8</v>
       </c>
       <c r="B27">
-        <v>1234567915</v>
+        <v>1234567937</v>
       </c>
       <c r="C27">
         <v>9</v>
       </c>
       <c r="D27">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -767,13 +767,13 @@
         <v>2</v>
       </c>
       <c r="B28">
-        <v>1234567916</v>
+        <v>1234567938</v>
       </c>
       <c r="C28">
         <v>9</v>
       </c>
       <c r="D28">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -781,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="B29">
-        <v>1234567917</v>
+        <v>1234567939</v>
       </c>
       <c r="C29">
         <v>9</v>
       </c>
       <c r="D29">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -795,21 +795,21 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>1234567918</v>
+        <v>1234567940</v>
       </c>
       <c r="C30">
         <v>9</v>
       </c>
       <c r="D30">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>4</v>
+      <c r="A31" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B31">
-        <v>1234567919</v>
+        <v>1234567941</v>
       </c>
       <c r="C31">
         <v>9</v>
@@ -819,11 +819,11 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
+      <c r="A32" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>1234567920</v>
+        <v>1234567942</v>
       </c>
       <c r="C32">
         <v>9</v>
@@ -833,11 +833,11 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>6</v>
+      <c r="A33" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B33">
-        <v>1234567921</v>
+        <v>1234567943</v>
       </c>
       <c r="C33">
         <v>9</v>
@@ -848,10 +848,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>1234567922</v>
+        <v>1234567944</v>
       </c>
       <c r="C34">
         <v>9</v>
@@ -862,10 +862,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B35">
-        <v>1234567923</v>
+        <v>1234567945</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -876,10 +876,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>1234567924</v>
+        <v>1234567946</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B37">
-        <v>1234567925</v>
+        <v>1234567947</v>
       </c>
       <c r="C37">
         <v>9</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>1234567926</v>
+        <v>1234567948</v>
       </c>
       <c r="C38">
         <v>9</v>
@@ -918,10 +918,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B39">
-        <v>1234567927</v>
+        <v>1234567949</v>
       </c>
       <c r="C39">
         <v>9</v>
@@ -931,11 +931,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
+      <c r="A40" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>1234567928</v>
+        <v>1234567950</v>
       </c>
       <c r="C40">
         <v>9</v>
@@ -945,11 +945,11 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>5</v>
+      <c r="A41" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B41">
-        <v>1234567929</v>
+        <v>1234567951</v>
       </c>
       <c r="C41">
         <v>9</v>
@@ -959,11 +959,11 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>6</v>
+      <c r="A42" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>1234567930</v>
+        <v>1234567952</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -974,10 +974,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B43">
-        <v>1234567931</v>
+        <v>1234567953</v>
       </c>
       <c r="C43">
         <v>9</v>
@@ -988,10 +988,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B44">
-        <v>1234567932</v>
+        <v>1234567954</v>
       </c>
       <c r="C44">
         <v>9</v>
@@ -1002,30 +1002,30 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B45">
-        <v>1234567933</v>
+        <v>1234567955</v>
       </c>
       <c r="C45">
         <v>9</v>
       </c>
       <c r="D45">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B46">
-        <v>1234567934</v>
+        <v>1234567956</v>
       </c>
       <c r="C46">
         <v>9</v>
       </c>
       <c r="D46">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1033,13 +1033,13 @@
         <v>0</v>
       </c>
       <c r="B47">
-        <v>1234567935</v>
+        <v>1234567957</v>
       </c>
       <c r="C47">
         <v>9</v>
       </c>
       <c r="D47">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1047,189 +1047,189 @@
         <v>3</v>
       </c>
       <c r="B48">
-        <v>1234567936</v>
+        <v>1234567958</v>
       </c>
       <c r="C48">
         <v>9</v>
       </c>
       <c r="D48">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>4</v>
+      <c r="A49" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B49">
-        <v>1234567937</v>
+        <v>1234567959</v>
       </c>
       <c r="C49">
         <v>9</v>
       </c>
       <c r="D49">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>5</v>
+      <c r="A50" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B50">
-        <v>1234567938</v>
+        <v>1234567960</v>
       </c>
       <c r="C50">
         <v>9</v>
       </c>
       <c r="D50">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>6</v>
+      <c r="A51" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B51">
-        <v>1234567939</v>
+        <v>1234567961</v>
       </c>
       <c r="C51">
         <v>9</v>
       </c>
       <c r="D51">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B52">
-        <v>1234567940</v>
+        <v>1234567962</v>
       </c>
       <c r="C52">
         <v>9</v>
       </c>
       <c r="D52">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B53">
-        <v>1234567941</v>
+        <v>1234567963</v>
       </c>
       <c r="C53">
         <v>9</v>
       </c>
       <c r="D53">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>1234567942</v>
+        <v>1234567964</v>
       </c>
       <c r="C54">
         <v>9</v>
       </c>
       <c r="D54">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B55">
-        <v>1234567943</v>
+        <v>1234567965</v>
       </c>
       <c r="C55">
         <v>9</v>
       </c>
       <c r="D55">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B56">
-        <v>1234567944</v>
+        <v>1234567966</v>
       </c>
       <c r="C56">
         <v>9</v>
       </c>
       <c r="D56">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B57">
-        <v>1234567945</v>
+        <v>1234567967</v>
       </c>
       <c r="C57">
         <v>9</v>
       </c>
       <c r="D57">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>4</v>
+      <c r="A58" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B58">
-        <v>1234567946</v>
+        <v>1234567968</v>
       </c>
       <c r="C58">
         <v>9</v>
       </c>
       <c r="D58">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>5</v>
+      <c r="A59" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B59">
-        <v>1234567947</v>
+        <v>1234567969</v>
       </c>
       <c r="C59">
         <v>9</v>
       </c>
       <c r="D59">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>6</v>
+      <c r="A60" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B60">
-        <v>1234567948</v>
+        <v>1234567970</v>
       </c>
       <c r="C60">
         <v>9</v>
       </c>
       <c r="D60">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61">
-        <v>1234567949</v>
+        <v>1234567971</v>
       </c>
       <c r="C61">
         <v>9</v>
@@ -1240,10 +1240,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B62">
-        <v>1234567950</v>
+        <v>1234567972</v>
       </c>
       <c r="C62">
         <v>9</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B63">
-        <v>1234567951</v>
+        <v>1234567973</v>
       </c>
       <c r="C63">
         <v>9</v>
@@ -1268,10 +1268,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B64">
-        <v>1234567952</v>
+        <v>1234567974</v>
       </c>
       <c r="C64">
         <v>9</v>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="B65">
-        <v>1234567953</v>
+        <v>1234567975</v>
       </c>
       <c r="C65">
         <v>9</v>
@@ -1299,7 +1299,7 @@
         <v>3</v>
       </c>
       <c r="B66">
-        <v>1234567954</v>
+        <v>1234567976</v>
       </c>
       <c r="C66">
         <v>9</v>
@@ -1309,227 +1309,227 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>4</v>
+      <c r="A67" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B67">
-        <v>1234567955</v>
+        <v>1234567977</v>
       </c>
       <c r="C67">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D67">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>5</v>
+      <c r="A68" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B68">
-        <v>1234567956</v>
+        <v>1234567978</v>
       </c>
       <c r="C68">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D68">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>6</v>
+      <c r="A69" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B69">
-        <v>1234567957</v>
+        <v>1234567979</v>
       </c>
       <c r="C69">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D69">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B70">
-        <v>1234567958</v>
+        <v>1234567980</v>
       </c>
       <c r="C70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D70">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B71">
-        <v>1234567959</v>
+        <v>1234567981</v>
       </c>
       <c r="C71">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D71">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B72">
-        <v>1234567960</v>
+        <v>1234567982</v>
       </c>
       <c r="C72">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D72">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B73">
-        <v>1234567961</v>
+        <v>1234567983</v>
       </c>
       <c r="C73">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D73">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B74">
-        <v>1234567962</v>
+        <v>1234567984</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D74">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B75">
-        <v>1234567963</v>
+        <v>1234567985</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D75">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>4</v>
+      <c r="A76" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B76">
-        <v>1234567964</v>
+        <v>1234567986</v>
       </c>
       <c r="C76">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D76">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>5</v>
+      <c r="A77" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B77">
-        <v>1234567965</v>
+        <v>1234567987</v>
       </c>
       <c r="C77">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D77">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>6</v>
+      <c r="A78" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B78">
-        <v>1234567966</v>
+        <v>1234567988</v>
       </c>
       <c r="C78">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D78">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B79">
-        <v>1234567967</v>
+        <v>1234567989</v>
       </c>
       <c r="C79">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D79">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B80">
-        <v>1234567968</v>
+        <v>1234567990</v>
       </c>
       <c r="C80">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D80">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B81">
-        <v>1234567969</v>
+        <v>1234567991</v>
       </c>
       <c r="C81">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D81">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B82">
-        <v>1234567970</v>
+        <v>1234567992</v>
       </c>
       <c r="C82">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D82">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1537,13 +1537,13 @@
         <v>0</v>
       </c>
       <c r="B83">
-        <v>1234567971</v>
+        <v>1234567993</v>
       </c>
       <c r="C83">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D83">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1551,428 +1551,2618 @@
         <v>3</v>
       </c>
       <c r="B84">
-        <v>1234567972</v>
+        <v>1234567994</v>
       </c>
       <c r="C84">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D84">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>4</v>
+      <c r="A85" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B85">
-        <v>1234567973</v>
+        <v>1234567995</v>
       </c>
       <c r="C85">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D85">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>5</v>
+      <c r="A86" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B86">
-        <v>1234567974</v>
+        <v>1234567996</v>
       </c>
       <c r="C86">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D86">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>6</v>
+      <c r="A87" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B87">
-        <v>1234567975</v>
+        <v>1234567997</v>
       </c>
       <c r="C87">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D87">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B88">
-        <v>1234567976</v>
+        <v>1234567998</v>
       </c>
       <c r="C88">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D88">
-        <v>801</v>
+        <v>903</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B89">
-        <v>1234567977</v>
+        <v>1234567999</v>
       </c>
       <c r="C89">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D89">
-        <v>802</v>
+        <v>903</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B90">
-        <v>1234567978</v>
+        <v>1234568000</v>
       </c>
       <c r="C90">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D90">
-        <v>802</v>
+        <v>903</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B91">
-        <v>1234567979</v>
+        <v>1234568001</v>
       </c>
       <c r="C91">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D91">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B92">
-        <v>1234567980</v>
+        <v>1234568002</v>
       </c>
       <c r="C92">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D92">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B93">
-        <v>1234567981</v>
+        <v>1234568003</v>
       </c>
       <c r="C93">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D93">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>4</v>
+      <c r="A94" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B94">
-        <v>1234567982</v>
+        <v>1234568004</v>
       </c>
       <c r="C94">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D94">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>5</v>
+      <c r="A95" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B95">
-        <v>1234567983</v>
+        <v>1234568005</v>
       </c>
       <c r="C95">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D95">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>6</v>
+      <c r="A96" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B96">
-        <v>1234567984</v>
+        <v>1234568006</v>
       </c>
       <c r="C96">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D96">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B97">
-        <v>1234567985</v>
+        <v>1234568007</v>
       </c>
       <c r="C97">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D97">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B98">
-        <v>1234567986</v>
+        <v>1234568008</v>
       </c>
       <c r="C98">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D98">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B99">
-        <v>1234567987</v>
+        <v>1234568009</v>
       </c>
       <c r="C99">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D99">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100">
+        <v>1234568010</v>
+      </c>
+      <c r="C100">
+        <v>9</v>
+      </c>
+      <c r="D100">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101">
+        <v>1234568011</v>
+      </c>
+      <c r="C101">
+        <v>9</v>
+      </c>
+      <c r="D101">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B102">
+        <v>1234568012</v>
+      </c>
+      <c r="C102">
+        <v>9</v>
+      </c>
+      <c r="D102">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B103">
+        <v>1234568013</v>
+      </c>
+      <c r="C103">
+        <v>9</v>
+      </c>
+      <c r="D103">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104">
+        <v>1234568014</v>
+      </c>
+      <c r="C104">
+        <v>9</v>
+      </c>
+      <c r="D104">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B105">
+        <v>1234568015</v>
+      </c>
+      <c r="C105">
+        <v>9</v>
+      </c>
+      <c r="D105">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106">
+        <v>1234568016</v>
+      </c>
+      <c r="C106">
+        <v>9</v>
+      </c>
+      <c r="D106">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B107">
+        <v>1234568017</v>
+      </c>
+      <c r="C107">
+        <v>9</v>
+      </c>
+      <c r="D107">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108">
+        <v>1234568018</v>
+      </c>
+      <c r="C108">
+        <v>9</v>
+      </c>
+      <c r="D108">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B109">
+        <v>1234568019</v>
+      </c>
+      <c r="C109">
+        <v>9</v>
+      </c>
+      <c r="D109">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>1234568020</v>
+      </c>
+      <c r="C110">
+        <v>9</v>
+      </c>
+      <c r="D110">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B111">
+        <v>1234568021</v>
+      </c>
+      <c r="C111">
+        <v>9</v>
+      </c>
+      <c r="D111">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <v>1234568022</v>
+      </c>
+      <c r="C112">
+        <v>9</v>
+      </c>
+      <c r="D112">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>1234568023</v>
+      </c>
+      <c r="C113">
+        <v>9</v>
+      </c>
+      <c r="D113">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B114">
+        <v>1234568024</v>
+      </c>
+      <c r="C114">
+        <v>9</v>
+      </c>
+      <c r="D114">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>1234568025</v>
+      </c>
+      <c r="C115">
+        <v>9</v>
+      </c>
+      <c r="D115">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <v>1234568026</v>
+      </c>
+      <c r="C116">
+        <v>9</v>
+      </c>
+      <c r="D116">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B117">
+        <v>1234568027</v>
+      </c>
+      <c r="C117">
+        <v>9</v>
+      </c>
+      <c r="D117">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>1234568028</v>
+      </c>
+      <c r="C118">
+        <v>9</v>
+      </c>
+      <c r="D118">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B119">
+        <v>1234568029</v>
+      </c>
+      <c r="C119">
+        <v>9</v>
+      </c>
+      <c r="D119">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>1234568030</v>
+      </c>
+      <c r="C120">
+        <v>9</v>
+      </c>
+      <c r="D120">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B121">
+        <v>1234568031</v>
+      </c>
+      <c r="C121">
+        <v>9</v>
+      </c>
+      <c r="D121">
         <v>802</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="1"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="1"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="1"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" s="1"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A107" s="1"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="1"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A109" s="1"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" s="1"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A111" s="1"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="1"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="1"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="1"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="1"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="1"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="1"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="1"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A165" s="1"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A169" s="1"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A170" s="1"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A171" s="1"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A173" s="1"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A174" s="1"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A178" s="1"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A180" s="1"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A181" s="1"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A182" s="1"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A183" s="1"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A187" s="1"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A188" s="1"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A189" s="1"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A190" s="1"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A191" s="1"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A196" s="1"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A197" s="1"/>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A198" s="1"/>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A199" s="1"/>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A200" s="1"/>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122">
+        <v>1234568032</v>
+      </c>
+      <c r="C122">
+        <v>9</v>
+      </c>
+      <c r="D122">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123">
+        <v>1234568033</v>
+      </c>
+      <c r="C123">
+        <v>9</v>
+      </c>
+      <c r="D123">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124">
+        <v>1234568034</v>
+      </c>
+      <c r="C124">
+        <v>9</v>
+      </c>
+      <c r="D124">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B125">
+        <v>1234568035</v>
+      </c>
+      <c r="C125">
+        <v>9</v>
+      </c>
+      <c r="D125">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126">
+        <v>1234568036</v>
+      </c>
+      <c r="C126">
+        <v>9</v>
+      </c>
+      <c r="D126">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127">
+        <v>1234568037</v>
+      </c>
+      <c r="C127">
+        <v>9</v>
+      </c>
+      <c r="D127">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128">
+        <v>1234568038</v>
+      </c>
+      <c r="C128">
+        <v>9</v>
+      </c>
+      <c r="D128">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B129">
+        <v>1234568039</v>
+      </c>
+      <c r="C129">
+        <v>9</v>
+      </c>
+      <c r="D129">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130">
+        <v>1234568040</v>
+      </c>
+      <c r="C130">
+        <v>9</v>
+      </c>
+      <c r="D130">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B131">
+        <v>1234568041</v>
+      </c>
+      <c r="C131">
+        <v>9</v>
+      </c>
+      <c r="D131">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132">
+        <v>1234568042</v>
+      </c>
+      <c r="C132">
+        <v>9</v>
+      </c>
+      <c r="D132">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B133">
+        <v>1234568043</v>
+      </c>
+      <c r="C133">
+        <v>9</v>
+      </c>
+      <c r="D133">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134">
+        <v>1234568044</v>
+      </c>
+      <c r="C134">
+        <v>9</v>
+      </c>
+      <c r="D134">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B135">
+        <v>1234568045</v>
+      </c>
+      <c r="C135">
+        <v>9</v>
+      </c>
+      <c r="D135">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136">
+        <v>1234568046</v>
+      </c>
+      <c r="C136">
+        <v>9</v>
+      </c>
+      <c r="D136">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B137">
+        <v>1234568047</v>
+      </c>
+      <c r="C137">
+        <v>9</v>
+      </c>
+      <c r="D137">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138">
+        <v>1234568048</v>
+      </c>
+      <c r="C138">
+        <v>9</v>
+      </c>
+      <c r="D138">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139">
+        <v>1234568049</v>
+      </c>
+      <c r="C139">
+        <v>9</v>
+      </c>
+      <c r="D139">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140">
+        <v>1234568050</v>
+      </c>
+      <c r="C140">
+        <v>9</v>
+      </c>
+      <c r="D140">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B141">
+        <v>1234568051</v>
+      </c>
+      <c r="C141">
+        <v>9</v>
+      </c>
+      <c r="D141">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142">
+        <v>1234568052</v>
+      </c>
+      <c r="C142">
+        <v>9</v>
+      </c>
+      <c r="D142">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143">
+        <v>1234568053</v>
+      </c>
+      <c r="C143">
+        <v>9</v>
+      </c>
+      <c r="D143">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144">
+        <v>1234568054</v>
+      </c>
+      <c r="C144">
+        <v>9</v>
+      </c>
+      <c r="D144">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145">
+        <v>1234568055</v>
+      </c>
+      <c r="C145">
+        <v>9</v>
+      </c>
+      <c r="D145">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146">
+        <v>1234568056</v>
+      </c>
+      <c r="C146">
+        <v>9</v>
+      </c>
+      <c r="D146">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B147">
+        <v>1234568057</v>
+      </c>
+      <c r="C147">
+        <v>9</v>
+      </c>
+      <c r="D147">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148">
+        <v>1234568058</v>
+      </c>
+      <c r="C148">
+        <v>9</v>
+      </c>
+      <c r="D148">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149">
+        <v>1234568059</v>
+      </c>
+      <c r="C149">
+        <v>9</v>
+      </c>
+      <c r="D149">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150">
+        <v>1234568060</v>
+      </c>
+      <c r="C150">
+        <v>9</v>
+      </c>
+      <c r="D150">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B151">
+        <v>1234568061</v>
+      </c>
+      <c r="C151">
+        <v>9</v>
+      </c>
+      <c r="D151">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>1234568062</v>
+      </c>
+      <c r="C152">
+        <v>9</v>
+      </c>
+      <c r="D152">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153">
+        <v>1234568063</v>
+      </c>
+      <c r="C153">
+        <v>9</v>
+      </c>
+      <c r="D153">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B154">
+        <v>1234568064</v>
+      </c>
+      <c r="C154">
+        <v>9</v>
+      </c>
+      <c r="D154">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155">
+        <v>1234568065</v>
+      </c>
+      <c r="C155">
+        <v>9</v>
+      </c>
+      <c r="D155">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156">
+        <v>1234568066</v>
+      </c>
+      <c r="C156">
+        <v>9</v>
+      </c>
+      <c r="D156">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B157">
+        <v>1234568067</v>
+      </c>
+      <c r="C157">
+        <v>9</v>
+      </c>
+      <c r="D157">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158">
+        <v>1234568068</v>
+      </c>
+      <c r="C158">
+        <v>9</v>
+      </c>
+      <c r="D158">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B159">
+        <v>1234568069</v>
+      </c>
+      <c r="C159">
+        <v>9</v>
+      </c>
+      <c r="D159">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160">
+        <v>1234568070</v>
+      </c>
+      <c r="C160">
+        <v>9</v>
+      </c>
+      <c r="D160">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161">
+        <v>1234568071</v>
+      </c>
+      <c r="C161">
+        <v>9</v>
+      </c>
+      <c r="D161">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162">
+        <v>1234568072</v>
+      </c>
+      <c r="C162">
+        <v>9</v>
+      </c>
+      <c r="D162">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B163">
+        <v>1234568073</v>
+      </c>
+      <c r="C163">
+        <v>9</v>
+      </c>
+      <c r="D163">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164">
+        <v>1234568074</v>
+      </c>
+      <c r="C164">
+        <v>9</v>
+      </c>
+      <c r="D164">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B165">
+        <v>1234568075</v>
+      </c>
+      <c r="C165">
+        <v>9</v>
+      </c>
+      <c r="D165">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166">
+        <v>1234568076</v>
+      </c>
+      <c r="C166">
+        <v>9</v>
+      </c>
+      <c r="D166">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B167">
+        <v>1234568077</v>
+      </c>
+      <c r="C167">
+        <v>9</v>
+      </c>
+      <c r="D167">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B168">
+        <v>1234568078</v>
+      </c>
+      <c r="C168">
+        <v>9</v>
+      </c>
+      <c r="D168">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169">
+        <v>1234568079</v>
+      </c>
+      <c r="C169">
+        <v>9</v>
+      </c>
+      <c r="D169">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170">
+        <v>1234568080</v>
+      </c>
+      <c r="C170">
+        <v>9</v>
+      </c>
+      <c r="D170">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171">
+        <v>1234568081</v>
+      </c>
+      <c r="C171">
+        <v>9</v>
+      </c>
+      <c r="D171">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172">
+        <v>1234568082</v>
+      </c>
+      <c r="C172">
+        <v>9</v>
+      </c>
+      <c r="D172">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173">
+        <v>1234568083</v>
+      </c>
+      <c r="C173">
+        <v>9</v>
+      </c>
+      <c r="D173">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174">
+        <v>1234568084</v>
+      </c>
+      <c r="C174">
+        <v>9</v>
+      </c>
+      <c r="D174">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175">
+        <v>1234568085</v>
+      </c>
+      <c r="C175">
+        <v>9</v>
+      </c>
+      <c r="D175">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176">
+        <v>1234568086</v>
+      </c>
+      <c r="C176">
+        <v>9</v>
+      </c>
+      <c r="D176">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177">
+        <v>1234568087</v>
+      </c>
+      <c r="C177">
+        <v>9</v>
+      </c>
+      <c r="D177">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178">
+        <v>1234568088</v>
+      </c>
+      <c r="C178">
+        <v>9</v>
+      </c>
+      <c r="D178">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179">
+        <v>1234568089</v>
+      </c>
+      <c r="C179">
+        <v>9</v>
+      </c>
+      <c r="D179">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180">
+        <v>1234568090</v>
+      </c>
+      <c r="C180">
+        <v>9</v>
+      </c>
+      <c r="D180">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B181">
+        <v>1234568091</v>
+      </c>
+      <c r="C181">
+        <v>9</v>
+      </c>
+      <c r="D181">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182">
+        <v>1234568092</v>
+      </c>
+      <c r="C182">
+        <v>9</v>
+      </c>
+      <c r="D182">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183">
+        <v>1234568093</v>
+      </c>
+      <c r="C183">
+        <v>9</v>
+      </c>
+      <c r="D183">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184">
+        <v>1234568094</v>
+      </c>
+      <c r="C184">
+        <v>9</v>
+      </c>
+      <c r="D184">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B185">
+        <v>1234568095</v>
+      </c>
+      <c r="C185">
+        <v>9</v>
+      </c>
+      <c r="D185">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186">
+        <v>1234568096</v>
+      </c>
+      <c r="C186">
+        <v>9</v>
+      </c>
+      <c r="D186">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B187">
+        <v>1234568097</v>
+      </c>
+      <c r="C187">
+        <v>9</v>
+      </c>
+      <c r="D187">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188">
+        <v>1234568098</v>
+      </c>
+      <c r="C188">
+        <v>9</v>
+      </c>
+      <c r="D188">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B189">
+        <v>1234568099</v>
+      </c>
+      <c r="C189">
+        <v>9</v>
+      </c>
+      <c r="D189">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190">
+        <v>1234568100</v>
+      </c>
+      <c r="C190">
+        <v>9</v>
+      </c>
+      <c r="D190">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B191">
+        <v>1234568101</v>
+      </c>
+      <c r="C191">
+        <v>9</v>
+      </c>
+      <c r="D191">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192">
+        <v>1234568102</v>
+      </c>
+      <c r="C192">
+        <v>9</v>
+      </c>
+      <c r="D192">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B193">
+        <v>1234568103</v>
+      </c>
+      <c r="C193">
+        <v>9</v>
+      </c>
+      <c r="D193">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194">
+        <v>1234568104</v>
+      </c>
+      <c r="C194">
+        <v>9</v>
+      </c>
+      <c r="D194">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B195">
+        <v>1234568105</v>
+      </c>
+      <c r="C195">
+        <v>9</v>
+      </c>
+      <c r="D195">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196">
+        <v>1234568106</v>
+      </c>
+      <c r="C196">
+        <v>9</v>
+      </c>
+      <c r="D196">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B197">
+        <v>1234568107</v>
+      </c>
+      <c r="C197">
+        <v>9</v>
+      </c>
+      <c r="D197">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198">
+        <v>1234568108</v>
+      </c>
+      <c r="C198">
+        <v>9</v>
+      </c>
+      <c r="D198">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B199">
+        <v>1234568109</v>
+      </c>
+      <c r="C199">
+        <v>9</v>
+      </c>
+      <c r="D199">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200">
+        <v>1234568110</v>
+      </c>
+      <c r="C200">
+        <v>9</v>
+      </c>
+      <c r="D200">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B201">
+        <v>1234568111</v>
+      </c>
+      <c r="C201">
+        <v>9</v>
+      </c>
+      <c r="D201">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202">
+        <v>1234568112</v>
+      </c>
+      <c r="C202">
+        <v>9</v>
+      </c>
+      <c r="D202">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B203">
+        <v>1234568113</v>
+      </c>
+      <c r="C203">
+        <v>9</v>
+      </c>
+      <c r="D203">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204">
+        <v>1234568114</v>
+      </c>
+      <c r="C204">
+        <v>9</v>
+      </c>
+      <c r="D204">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B205">
+        <v>1234568115</v>
+      </c>
+      <c r="C205">
+        <v>9</v>
+      </c>
+      <c r="D205">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206">
+        <v>1234568116</v>
+      </c>
+      <c r="C206">
+        <v>9</v>
+      </c>
+      <c r="D206">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B207">
+        <v>1234568117</v>
+      </c>
+      <c r="C207">
+        <v>9</v>
+      </c>
+      <c r="D207">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>1234568118</v>
+      </c>
+      <c r="C208">
+        <v>9</v>
+      </c>
+      <c r="D208">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B209">
+        <v>1234568119</v>
+      </c>
+      <c r="C209">
+        <v>9</v>
+      </c>
+      <c r="D209">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210">
+        <v>1234568120</v>
+      </c>
+      <c r="C210">
+        <v>9</v>
+      </c>
+      <c r="D210">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B211">
+        <v>1234568121</v>
+      </c>
+      <c r="C211">
+        <v>9</v>
+      </c>
+      <c r="D211">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212">
+        <v>1234568122</v>
+      </c>
+      <c r="C212">
+        <v>9</v>
+      </c>
+      <c r="D212">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213">
+        <v>1234568123</v>
+      </c>
+      <c r="C213">
+        <v>9</v>
+      </c>
+      <c r="D213">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B214">
+        <v>1234568124</v>
+      </c>
+      <c r="C214">
+        <v>9</v>
+      </c>
+      <c r="D214">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B215">
+        <v>1234568125</v>
+      </c>
+      <c r="C215">
+        <v>9</v>
+      </c>
+      <c r="D215">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B216">
+        <v>1234568126</v>
+      </c>
+      <c r="C216">
+        <v>9</v>
+      </c>
+      <c r="D216">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B217">
+        <v>1234568127</v>
+      </c>
+      <c r="C217">
+        <v>9</v>
+      </c>
+      <c r="D217">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218">
+        <v>1234568128</v>
+      </c>
+      <c r="C218">
+        <v>9</v>
+      </c>
+      <c r="D218">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B219">
+        <v>1234568129</v>
+      </c>
+      <c r="C219">
+        <v>9</v>
+      </c>
+      <c r="D219">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B220">
+        <v>1234568130</v>
+      </c>
+      <c r="C220">
+        <v>9</v>
+      </c>
+      <c r="D220">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B221">
+        <v>1234568131</v>
+      </c>
+      <c r="C221">
+        <v>9</v>
+      </c>
+      <c r="D221">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B222">
+        <v>1234568132</v>
+      </c>
+      <c r="C222">
+        <v>9</v>
+      </c>
+      <c r="D222">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223">
+        <v>1234568133</v>
+      </c>
+      <c r="C223">
+        <v>9</v>
+      </c>
+      <c r="D223">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B224">
+        <v>1234568134</v>
+      </c>
+      <c r="C224">
+        <v>9</v>
+      </c>
+      <c r="D224">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B225">
+        <v>1234568135</v>
+      </c>
+      <c r="C225">
+        <v>9</v>
+      </c>
+      <c r="D225">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B226">
+        <v>1234568136</v>
+      </c>
+      <c r="C226">
+        <v>9</v>
+      </c>
+      <c r="D226">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B227">
+        <v>1234568137</v>
+      </c>
+      <c r="C227">
+        <v>9</v>
+      </c>
+      <c r="D227">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228">
+        <v>1234568138</v>
+      </c>
+      <c r="C228">
+        <v>9</v>
+      </c>
+      <c r="D228">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B229">
+        <v>1234568139</v>
+      </c>
+      <c r="C229">
+        <v>9</v>
+      </c>
+      <c r="D229">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B230">
+        <v>1234568140</v>
+      </c>
+      <c r="C230">
+        <v>9</v>
+      </c>
+      <c r="D230">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B231">
+        <v>1234568141</v>
+      </c>
+      <c r="C231">
+        <v>9</v>
+      </c>
+      <c r="D231">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B232">
+        <v>1234568142</v>
+      </c>
+      <c r="C232">
+        <v>9</v>
+      </c>
+      <c r="D232">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B233">
+        <v>1234568143</v>
+      </c>
+      <c r="C233">
+        <v>9</v>
+      </c>
+      <c r="D233">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B234">
+        <v>1234568144</v>
+      </c>
+      <c r="C234">
+        <v>9</v>
+      </c>
+      <c r="D234">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B235">
+        <v>1234568145</v>
+      </c>
+      <c r="C235">
+        <v>9</v>
+      </c>
+      <c r="D235">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236">
+        <v>1234568146</v>
+      </c>
+      <c r="C236">
+        <v>9</v>
+      </c>
+      <c r="D236">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237">
+        <v>1234568147</v>
+      </c>
+      <c r="C237">
+        <v>9</v>
+      </c>
+      <c r="D237">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238">
+        <v>1234568148</v>
+      </c>
+      <c r="C238">
+        <v>9</v>
+      </c>
+      <c r="D238">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B239">
+        <v>1234568149</v>
+      </c>
+      <c r="C239">
+        <v>9</v>
+      </c>
+      <c r="D239">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B240">
+        <v>1234568150</v>
+      </c>
+      <c r="C240">
+        <v>9</v>
+      </c>
+      <c r="D240">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241">
+        <v>1234568151</v>
+      </c>
+      <c r="C241">
+        <v>9</v>
+      </c>
+      <c r="D241">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242">
+        <v>1234568152</v>
+      </c>
+      <c r="C242">
+        <v>9</v>
+      </c>
+      <c r="D242">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B243">
+        <v>1234568153</v>
+      </c>
+      <c r="C243">
+        <v>9</v>
+      </c>
+      <c r="D243">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B244">
+        <v>1234568154</v>
+      </c>
+      <c r="C244">
+        <v>9</v>
+      </c>
+      <c r="D244">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B245">
+        <v>1234568155</v>
+      </c>
+      <c r="C245">
+        <v>9</v>
+      </c>
+      <c r="D245">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246">
+        <v>1234568156</v>
+      </c>
+      <c r="C246">
+        <v>9</v>
+      </c>
+      <c r="D246">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247">
+        <v>1234568157</v>
+      </c>
+      <c r="C247">
+        <v>9</v>
+      </c>
+      <c r="D247">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B248">
+        <v>1234568158</v>
+      </c>
+      <c r="C248">
+        <v>9</v>
+      </c>
+      <c r="D248">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B249">
+        <v>1234568159</v>
+      </c>
+      <c r="C249">
+        <v>9</v>
+      </c>
+      <c r="D249">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B250">
+        <v>1234568160</v>
+      </c>
+      <c r="C250">
+        <v>9</v>
+      </c>
+      <c r="D250">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B251">
+        <v>1234568161</v>
+      </c>
+      <c r="C251">
+        <v>9</v>
+      </c>
+      <c r="D251">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B252">
+        <v>1234568162</v>
+      </c>
+      <c r="C252">
+        <v>9</v>
+      </c>
+      <c r="D252">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253">
+        <v>1234568163</v>
+      </c>
+      <c r="C253">
+        <v>9</v>
+      </c>
+      <c r="D253">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254">
+        <v>1234568164</v>
+      </c>
+      <c r="C254">
+        <v>9</v>
+      </c>
+      <c r="D254">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B255">
+        <v>1234568165</v>
+      </c>
+      <c r="C255">
+        <v>9</v>
+      </c>
+      <c r="D255">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B256">
+        <v>1234568166</v>
+      </c>
+      <c r="C256">
+        <v>9</v>
+      </c>
+      <c r="D256">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A257" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257">
+        <v>1234568167</v>
+      </c>
+      <c r="C257">
+        <v>9</v>
+      </c>
+      <c r="D257">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258">
+        <v>1234568168</v>
+      </c>
+      <c r="C258">
+        <v>9</v>
+      </c>
+      <c r="D258">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259">
+        <v>1234568169</v>
+      </c>
+      <c r="C259">
+        <v>9</v>
+      </c>
+      <c r="D259">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260">
+        <v>1234568170</v>
+      </c>
+      <c r="C260">
+        <v>9</v>
+      </c>
+      <c r="D260">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B261">
+        <v>1234568171</v>
+      </c>
+      <c r="C261">
+        <v>9</v>
+      </c>
+      <c r="D261">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B262">
+        <v>1234568172</v>
+      </c>
+      <c r="C262">
+        <v>9</v>
+      </c>
+      <c r="D262">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B263">
+        <v>1234568173</v>
+      </c>
+      <c r="C263">
+        <v>9</v>
+      </c>
+      <c r="D263">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264">
+        <v>1234568174</v>
+      </c>
+      <c r="C264">
+        <v>9</v>
+      </c>
+      <c r="D264">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B265">
+        <v>1234568175</v>
+      </c>
+      <c r="C265">
+        <v>9</v>
+      </c>
+      <c r="D265">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B266">
+        <v>1234568176</v>
+      </c>
+      <c r="C266">
+        <v>9</v>
+      </c>
+      <c r="D266">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267">
+        <v>1234568177</v>
+      </c>
+      <c r="C267">
+        <v>9</v>
+      </c>
+      <c r="D267">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B268">
+        <v>1234568178</v>
+      </c>
+      <c r="C268">
+        <v>9</v>
+      </c>
+      <c r="D268">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269">
+        <v>1234568179</v>
+      </c>
+      <c r="C269">
+        <v>9</v>
+      </c>
+      <c r="D269">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270">
+        <v>1234568180</v>
+      </c>
+      <c r="C270">
+        <v>9</v>
+      </c>
+      <c r="D270">
+        <v>703</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>